<commit_message>
Updating the table with simulation params
</commit_message>
<xml_diff>
--- a/references/IOTC-2024-TCAC13-REF03 - Simulation parameters.xlsx
+++ b/references/IOTC-2024-TCAC13-REF03 - Simulation parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ffiorellato\Desktop\TCAC simulations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dev\git\BitBucket workspaces\IOTC-ws\IOTC working parties\iotc-tcac-simulations\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70588130-7A25-4BBF-AED6-DA33935D64C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511464A2-F965-4228-94E0-FF8837E037C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C781CF1E-3B4F-4AFA-9DA3-CA2C4F64D35A}"/>
+    <workbookView xWindow="28680" yWindow="1140" windowWidth="29040" windowHeight="15720" xr2:uid="{C781CF1E-3B4F-4AFA-9DA3-CA2C4F64D35A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>Baseline</t>
   </si>
@@ -126,6 +126,18 @@
   </si>
   <si>
     <t>EEZ catches allocation (para. 6.8(2))</t>
+  </si>
+  <si>
+    <t>ZAF</t>
+  </si>
+  <si>
+    <t>0-100%</t>
+  </si>
+  <si>
+    <t>15-40%</t>
+  </si>
+  <si>
+    <t>60-80%</t>
   </si>
 </sst>
 </file>
@@ -165,7 +177,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,12 +190,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="50">
     <border>
@@ -822,7 +828,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -904,146 +910,176 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1362,7 +1398,7 @@
   <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:T1"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1377,67 +1413,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51"/>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="51"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="73"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="53"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="52" t="s">
+      <c r="E2" s="75"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="55"/>
-      <c r="I2" s="83" t="s">
+      <c r="H2" s="77"/>
+      <c r="I2" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
-      <c r="P2" s="84"/>
-      <c r="Q2" s="84"/>
-      <c r="R2" s="84"/>
-      <c r="S2" s="84"/>
-      <c r="T2" s="85"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="48"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="49"/>
     </row>
     <row r="3" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="57"/>
-      <c r="B3" s="59"/>
-      <c r="C3" s="57"/>
+      <c r="A3" s="79"/>
+      <c r="B3" s="81"/>
+      <c r="C3" s="79"/>
       <c r="D3" s="29" t="s">
         <v>0</v>
       </c>
@@ -1491,13 +1527,13 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="57" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="26">
         <v>1</v>
       </c>
-      <c r="C4" s="67">
+      <c r="C4" s="60">
         <v>45288</v>
       </c>
       <c r="D4" s="16">
@@ -1509,55 +1545,55 @@
       <c r="F4" s="17">
         <v>0.8</v>
       </c>
-      <c r="G4" s="47">
+      <c r="G4" s="50">
         <v>0.1</v>
       </c>
-      <c r="H4" s="70">
+      <c r="H4" s="63">
         <v>0.9</v>
       </c>
-      <c r="I4" s="47" t="s">
+      <c r="I4" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="45">
+      <c r="J4" s="53">
         <v>10</v>
       </c>
-      <c r="K4" s="73">
+      <c r="K4" s="66">
         <v>0.1</v>
       </c>
-      <c r="L4" s="61">
+      <c r="L4" s="41">
         <v>0.2</v>
       </c>
-      <c r="M4" s="61">
+      <c r="M4" s="41">
         <v>0.3</v>
       </c>
-      <c r="N4" s="61">
+      <c r="N4" s="41">
         <v>0.4</v>
       </c>
-      <c r="O4" s="61">
+      <c r="O4" s="41">
         <v>0.5</v>
       </c>
-      <c r="P4" s="61">
+      <c r="P4" s="41">
         <v>0.6</v>
       </c>
-      <c r="Q4" s="61">
+      <c r="Q4" s="41">
         <v>0.7</v>
       </c>
-      <c r="R4" s="61">
+      <c r="R4" s="41">
         <v>0.8</v>
       </c>
-      <c r="S4" s="61">
+      <c r="S4" s="41">
         <v>0.9</v>
       </c>
-      <c r="T4" s="80">
+      <c r="T4" s="44">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="65"/>
+      <c r="A5" s="58"/>
       <c r="B5" s="27">
         <v>2</v>
       </c>
-      <c r="C5" s="65"/>
+      <c r="C5" s="58"/>
       <c r="D5" s="12">
         <v>0.1</v>
       </c>
@@ -1567,27 +1603,27 @@
       <c r="F5" s="14">
         <v>0.7</v>
       </c>
-      <c r="G5" s="68"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="86"/>
-      <c r="J5" s="87"/>
-      <c r="K5" s="74"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="62"/>
-      <c r="N5" s="62"/>
-      <c r="O5" s="62"/>
-      <c r="P5" s="62"/>
-      <c r="Q5" s="62"/>
-      <c r="R5" s="62"/>
-      <c r="S5" s="62"/>
-      <c r="T5" s="81"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="67"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
+      <c r="N5" s="42"/>
+      <c r="O5" s="42"/>
+      <c r="P5" s="42"/>
+      <c r="Q5" s="42"/>
+      <c r="R5" s="42"/>
+      <c r="S5" s="42"/>
+      <c r="T5" s="45"/>
     </row>
     <row r="6" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="66"/>
+      <c r="A6" s="59"/>
       <c r="B6" s="28">
         <v>3</v>
       </c>
-      <c r="C6" s="66"/>
+      <c r="C6" s="59"/>
       <c r="D6" s="18">
         <v>0.1</v>
       </c>
@@ -1597,29 +1633,29 @@
       <c r="F6" s="20">
         <v>0.6</v>
       </c>
-      <c r="G6" s="69"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="75"/>
-      <c r="L6" s="63"/>
-      <c r="M6" s="63"/>
-      <c r="N6" s="63"/>
-      <c r="O6" s="63"/>
-      <c r="P6" s="63"/>
-      <c r="Q6" s="63"/>
-      <c r="R6" s="63"/>
-      <c r="S6" s="63"/>
-      <c r="T6" s="82"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="68"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="43"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="43"/>
+      <c r="P6" s="43"/>
+      <c r="Q6" s="43"/>
+      <c r="R6" s="43"/>
+      <c r="S6" s="43"/>
+      <c r="T6" s="46"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="57" t="s">
         <v>28</v>
       </c>
       <c r="B7" s="26">
         <v>1</v>
       </c>
-      <c r="C7" s="67">
+      <c r="C7" s="60">
         <v>45267</v>
       </c>
       <c r="D7" s="16">
@@ -1631,53 +1667,55 @@
       <c r="F7" s="17">
         <v>0.65</v>
       </c>
-      <c r="G7" s="47">
-        <v>1</v>
-      </c>
-      <c r="H7" s="77">
+      <c r="G7" s="50">
+        <v>1</v>
+      </c>
+      <c r="H7" s="70">
         <v>0</v>
       </c>
-      <c r="I7" s="79" t="s">
+      <c r="I7" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="J7" s="45">
+      <c r="J7" s="53">
         <v>9</v>
       </c>
-      <c r="K7" s="47">
+      <c r="K7" s="50">
         <v>0.33</v>
       </c>
-      <c r="L7" s="43">
+      <c r="L7" s="82">
         <v>0.33</v>
       </c>
-      <c r="M7" s="49">
+      <c r="M7" s="84">
         <v>0.33</v>
       </c>
-      <c r="N7" s="43">
+      <c r="N7" s="82">
         <v>0.66</v>
       </c>
-      <c r="O7" s="43">
+      <c r="O7" s="82">
         <v>0.66</v>
       </c>
-      <c r="P7" s="43">
+      <c r="P7" s="82">
         <v>0.66</v>
       </c>
-      <c r="Q7" s="43">
-        <v>1</v>
-      </c>
-      <c r="R7" s="43">
-        <v>1</v>
-      </c>
-      <c r="S7" s="43">
-        <v>1</v>
-      </c>
-      <c r="T7" s="41"/>
+      <c r="Q7" s="82">
+        <v>1</v>
+      </c>
+      <c r="R7" s="82">
+        <v>1</v>
+      </c>
+      <c r="S7" s="82">
+        <v>1</v>
+      </c>
+      <c r="T7" s="70">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="66"/>
+      <c r="A8" s="59"/>
       <c r="B8" s="28">
         <v>2</v>
       </c>
-      <c r="C8" s="76"/>
+      <c r="C8" s="69"/>
       <c r="D8" s="40">
         <v>0.1</v>
       </c>
@@ -1687,86 +1725,164 @@
       <c r="F8" s="20">
         <v>0.7</v>
       </c>
-      <c r="G8" s="48"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="46"/>
-      <c r="K8" s="48"/>
-      <c r="L8" s="44"/>
-      <c r="M8" s="50"/>
-      <c r="N8" s="44"/>
-      <c r="O8" s="44"/>
-      <c r="P8" s="44"/>
-      <c r="Q8" s="44"/>
-      <c r="R8" s="44"/>
-      <c r="S8" s="44"/>
-      <c r="T8" s="42"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="52"/>
+      <c r="L8" s="83"/>
+      <c r="M8" s="85"/>
+      <c r="N8" s="83"/>
+      <c r="O8" s="83"/>
+      <c r="P8" s="83"/>
+      <c r="Q8" s="83"/>
+      <c r="R8" s="83"/>
+      <c r="S8" s="83"/>
+      <c r="T8" s="71"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="11"/>
+      <c r="A9" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="26">
+        <v>1</v>
+      </c>
+      <c r="C9" s="86">
+        <v>45290</v>
+      </c>
+      <c r="D9" s="88" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="89" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="90" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="16">
+        <v>1</v>
+      </c>
+      <c r="H9" s="93">
+        <v>0</v>
+      </c>
+      <c r="I9" s="88" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="96">
+        <v>5</v>
+      </c>
+      <c r="K9" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="L9" s="39">
+        <v>0.7</v>
+      </c>
+      <c r="M9" s="39">
+        <v>0.8</v>
+      </c>
+      <c r="N9" s="39">
+        <v>0.9</v>
+      </c>
+      <c r="O9" s="39">
+        <v>1</v>
+      </c>
+      <c r="P9" s="39">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="39">
+        <v>1</v>
+      </c>
+      <c r="R9" s="39">
+        <v>1</v>
+      </c>
+      <c r="S9" s="39">
+        <v>1</v>
+      </c>
+      <c r="T9" s="17">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="4"/>
+    <row r="10" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="59"/>
+      <c r="B10" s="28">
+        <v>2</v>
+      </c>
+      <c r="C10" s="87">
+        <v>45308</v>
+      </c>
+      <c r="D10" s="40">
+        <v>0.05</v>
+      </c>
+      <c r="E10" s="91" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="92" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="40">
+        <v>1</v>
+      </c>
+      <c r="H10" s="94">
+        <v>0</v>
+      </c>
+      <c r="I10" s="95" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="97">
+        <v>5</v>
+      </c>
+      <c r="K10" s="40">
+        <v>0.5</v>
+      </c>
+      <c r="L10" s="19">
+        <v>0.7</v>
+      </c>
+      <c r="M10" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="N10" s="19">
+        <v>0.9</v>
+      </c>
+      <c r="O10" s="19">
+        <v>1</v>
+      </c>
+      <c r="P10" s="19">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="19">
+        <v>1</v>
+      </c>
+      <c r="R10" s="19">
+        <v>1</v>
+      </c>
+      <c r="S10" s="19">
+        <v>1</v>
+      </c>
+      <c r="T10" s="20">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="4"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="11"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="24"/>
@@ -1843,23 +1959,34 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="60" t="s">
+      <c r="A17" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="60"/>
+      <c r="B17" s="56"/>
       <c r="C17" s="36">
-        <v>45299</v>
+        <v>45323</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="40">
-    <mergeCell ref="S4:S6"/>
-    <mergeCell ref="T4:T6"/>
-    <mergeCell ref="I2:T2"/>
-    <mergeCell ref="I4:I6"/>
-    <mergeCell ref="J4:J6"/>
-    <mergeCell ref="Q4:Q6"/>
-    <mergeCell ref="R4:R6"/>
+  <mergeCells count="41">
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="T7:T8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="S7:S8"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="B2:B3"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="M4:M6"/>
     <mergeCell ref="N4:N6"/>
@@ -1876,23 +2003,13 @@
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="I7:I8"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="S7:S8"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="Q7:Q8"/>
-    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="S4:S6"/>
+    <mergeCell ref="T4:T6"/>
+    <mergeCell ref="I2:T2"/>
+    <mergeCell ref="I4:I6"/>
+    <mergeCell ref="J4:J6"/>
+    <mergeCell ref="Q4:Q6"/>
+    <mergeCell ref="R4:R6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>